<commit_message>
built in linear model
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mutasim\Downloads\Projects\VendingPredictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7BA1EB-8DD0-46FF-A7A5-4C01E3A46129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AFE0CA-6847-478F-B8BA-BE35F783F0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="4065" windowWidth="14400" windowHeight="8100" xr2:uid="{07CBA644-BB9F-47AF-926D-6BE992C464A0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{07CBA644-BB9F-47AF-926D-6BE992C464A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0697DFB0-755D-4FED-A601-936D9308AD5B}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,17 +422,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>2.1800000000000002</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1978</v>
       </c>
       <c r="B2">
-        <f>B1+2</f>
-        <v>4.18</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,8 +436,8 @@
         <v>1979</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B18" si="0">B2+2</f>
-        <v>6.18</v>
+        <f>B2+2</f>
+        <v>4.18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,8 +445,8 @@
         <v>1980</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>8.18</v>
+        <f t="shared" ref="B4:B16" si="0">B3+2</f>
+        <v>6.18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -459,7 +455,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>10.18</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +464,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>12.18</v>
+        <v>10.18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,7 +473,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>14.18</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +482,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>16.18</v>
+        <v>14.18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,7 +491,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>18.18</v>
+        <v>16.18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,7 +500,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>20.18</v>
+        <v>18.18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +509,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>22.18</v>
+        <v>20.18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,7 +518,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>24.18</v>
+        <v>22.18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +527,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>26.18</v>
+        <v>24.18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +536,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>28.18</v>
+        <v>26.18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -549,7 +545,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>30.18</v>
+        <v>28.18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -558,7 +554,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>32.18</v>
+        <v>30.18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -566,8 +562,8 @@
         <v>1993</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>34.18</v>
+        <f>B16+2</f>
+        <v>32.18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -575,13 +571,17 @@
         <v>1994</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>36.18</v>
+        <f>B17+2</f>
+        <v>34.18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1995</v>
+      </c>
+      <c r="B19">
+        <f>B18+2</f>
+        <v>36.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>